<commit_message>
Save the forest plots, conduct three statistic tests of publication bias
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuhe/Desktop/meta analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuhe/Desktop/meta analysis/BPA_cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECA557A-9395-874C-9B0D-7980C9C77083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B6531-4672-2D49-B6EA-B4D6DEBABA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="20" windowWidth="21600" windowHeight="17320" xr2:uid="{AA13BBBF-42C7-FA48-89F4-239E5D59F49B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
     <t>Auther</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,10 @@
   </si>
   <si>
     <t>Duan31_mult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stro</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1266,7 +1270,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
finish the results table
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuhe/Desktop/meta analysis/BPA_cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B6531-4672-2D49-B6EA-B4D6DEBABA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B28E3BD-D334-AC4E-9FC7-A85BD2E77687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="20" windowWidth="21600" windowHeight="17320" xr2:uid="{AA13BBBF-42C7-FA48-89F4-239E5D59F49B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="18540" windowHeight="20360" activeTab="1" xr2:uid="{AA13BBBF-42C7-FA48-89F4-239E5D59F49B}"/>
   </bookViews>
   <sheets>
     <sheet name="strong_or" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="47">
   <si>
     <t>Auther</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,14 +56,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>subject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cancer type, 0 = breat cancer, 1 = prostate cancer, 2 = colorectal cancer, 3 = thyroid cancer, 4 = cervical, 5 = ovarian, 6 = uterine, 7 = Biliary Tract Cancer, 8 = lung cancer, 9 = osteosarcoma, 10 = Meningioma &amp; Glioma, 11 = glioma</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -80,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Wu2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Hawaii &amp; CA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +221,10 @@
   </si>
   <si>
     <t>stro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wu2_multi</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908E04EE-10E8-114E-8322-FB1ABBA28B3B}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:I24"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -641,30 +633,30 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -690,10 +682,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -719,10 +711,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -748,10 +740,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -777,10 +769,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -806,10 +798,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -835,10 +827,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -864,10 +856,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -893,10 +885,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -922,10 +914,10 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -951,10 +943,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -980,10 +972,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1009,10 +1001,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1038,10 +1030,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1067,10 +1059,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1096,10 +1088,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1125,10 +1117,10 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1154,10 +1146,10 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1183,10 +1175,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1212,10 +1204,10 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1241,10 +1233,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1270,10 +1262,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1299,10 +1291,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1336,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB8BC55-2692-704B-8F69-504BFC8D0ABC}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1353,30 +1345,30 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1402,10 +1394,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1431,10 +1423,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1460,10 +1452,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1489,10 +1481,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1518,10 +1510,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1547,10 +1539,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1576,10 +1568,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1605,10 +1597,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1634,10 +1626,10 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1663,10 +1655,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1692,10 +1684,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1721,10 +1713,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1750,10 +1742,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1779,10 +1771,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1808,10 +1800,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1837,10 +1829,10 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1866,10 +1858,10 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1895,10 +1887,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1924,10 +1916,10 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1953,10 +1945,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1982,10 +1974,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2011,10 +2003,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2061,27 +2053,27 @@
     </row>
     <row r="2" spans="1:1" ht="27" customHeight="1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="34" customHeight="1">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="54" customHeight="1">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>